<commit_message>
rm cds patient dfa4eb0e8863edf50712318255ab1a4039d580a3
</commit_message>
<xml_diff>
--- a/nr-test-delete-patient/ig/StructureDefinition-cds-ihe-careteam.xlsx
+++ b/nr-test-delete-patient/ig/StructureDefinition-cds-ihe-careteam.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1939" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1931" uniqueCount="381">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-29T07:49:03+00:00</t>
+    <t>2024-05-31T07:57:02+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -266,7 +266,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
     <t>Entity. Role, or Act</t>
@@ -313,17 +313,10 @@
     <t>Resource.meta</t>
   </si>
   <si>
-    <t xml:space="preserve">ele-1
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>CareTeam.meta.id</t>
   </si>
   <si>
@@ -481,12 +474,6 @@
     <t>Meta.security</t>
   </si>
   <si>
-    <t>CE/CNE/CWE subset one of the sets of component 1-3 or 4-6</t>
-  </si>
-  <si>
-    <t>CV</t>
-  </si>
-  <si>
     <t>CareTeam.meta.tag</t>
   </si>
   <si>
@@ -603,6 +590,9 @@
     <t>DomainResource.contained</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>CareTeam.extension</t>
   </si>
   <si>
@@ -650,12 +640,6 @@
     <t>FiveWs.identifier</t>
   </si>
   <si>
-    <t>CX / EI (occasionally, more often EI maps to a resource id or a URL)</t>
-  </si>
-  <si>
-    <t>II - The Identifier class is a little looser than the v3 type II because it allows URIs as well as registered OIDs or GUIDs.  Also maps to Role[classCode=IDENT]</t>
-  </si>
-  <si>
     <t>CareTeam.identifier.id</t>
   </si>
   <si>
@@ -790,15 +774,7 @@
     <t>Time period during which identifier is/was valid for use.</t>
   </si>
   <si>
-    <t>A Period specifies a range of time; the context of use will specify whether the entire range applies (e.g. "the patient was an inpatient of the hospital for this time range") or one value from the range applies (e.g. "give to the patient between these two times").
-Period is not used for a duration (a measure of elapsed time). See [Duration](http://hl7.org/fhir/R4/datatypes.html#Duration).</t>
-  </si>
-  <si>
     <t>Identifier.period</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-per-1:If present, start SHALL have a lower value than end {start.hasValue().not() or end.hasValue().not() or (start &lt;= end)}</t>
   </si>
   <si>
     <t>CX.7 + CX.8</t>
@@ -826,10 +802,6 @@
     <t>Identifier.assigner</t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ref-1:SHALL have a contained resource if a local reference is provided {reference.startsWith('#').not() or (reference.substring(1).trace('url') in %rootResource.contained.id.trace('ids'))}</t>
-  </si>
-  <si>
     <t>CX.4 / (CX.4,CX.9,CX.10)</t>
   </si>
   <si>
@@ -882,12 +854,6 @@
     <t>FiveWs.class</t>
   </si>
   <si>
-    <t>CE/CNE/CWE</t>
-  </si>
-  <si>
-    <t>CD</t>
-  </si>
-  <si>
     <t>CareTeam.name</t>
   </si>
   <si>
@@ -917,9 +883,6 @@
     <t>Identifies the patient or group whose intended care is handled by the team.</t>
   </si>
   <si>
-    <t>References SHALL be a reference to an actual FHIR resource, and SHALL be resolveable (allowing for access control, temporary unavailability, etc.). Resolution can be either by retrieval from the URL, or, where applicable by resource type, by treating an absolute reference as a canonical URL and looking it up in a local registry/repository.</t>
-  </si>
-  <si>
     <t>Allows the team to care for a group (e.g. marriage) therapy. 
 Allows for an organization to designate a team such as the PICC line team.</t>
   </si>
@@ -927,9 +890,6 @@
     <t>FiveWs.subject</t>
   </si>
   <si>
-    <t>The target of a resource reference is a RIM entry point (Act, Role, or Entity)</t>
-  </si>
-  <si>
     <t>CareTeam.encounter</t>
   </si>
   <si>
@@ -964,12 +924,6 @@
     <t>FiveWs.init</t>
   </si>
   <si>
-    <t>DR</t>
-  </si>
-  <si>
-    <t>IVL&lt;TS&gt;[lowClosed="true" and highClosed="true"] or URG&lt;TS&gt;[lowClosed="true" and highClosed="true"]</t>
-  </si>
-  <si>
     <t>CareTeam.period.id</t>
   </si>
   <si>
@@ -995,8 +949,8 @@
     <t>Period.start</t>
   </si>
   <si>
-    <t>ele-1
-per-1</t>
+    <t xml:space="preserve">per-1
+</t>
   </si>
   <si>
     <t>DR.1</t>
@@ -1045,12 +999,12 @@
     <t>It is possible for a care team to be set up with roles specified only, before actual participants are invited into or identified as team members</t>
   </si>
   <si>
-    <t>ele-1
-ctm-1</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ctm-1:CareTeam.participant.onBehalfOf can only be populated when CareTeam.participant.member is a Practitioner {onBehalfOf.exists() implies (member.resolve().iif(empty(), true, ofType(Practitioner).exists()))}</t>
+    <t xml:space="preserve">ctm-1
+</t>
+  </si>
+  <si>
+    <t>ctm-1:CareTeam.participant.onBehalfOf can only be populated when CareTeam.participant.member is a Practitioner {onBehalfOf.exists() implies (member.resolve().iif(empty(), true, ofType(Practitioner).exists()))}
+ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}</t>
   </si>
   <si>
     <t>REL (REL.4 is always the Patient) ( or PRT?)</t>
@@ -1190,9 +1144,6 @@
     <t>Describes why the care team exists.</t>
   </si>
   <si>
-    <t>Not all terminology uses fit this general pattern. In some cases, models should not use CodeableConcept and use Coding directly and provide their own structure for managing text, codings, translations and the relationship between elements and pre- and post-coordination.</t>
-  </si>
-  <si>
     <t>Indicates the reason for the care team.</t>
   </si>
   <si>
@@ -1240,16 +1191,6 @@
     <t>The ContactPoint.use code of home is not appropriate to use. These contacts are not the contact details of individual care team members.</t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-cpt-2:A system is required if a value is provided. {value.empty() or system.exists()}</t>
-  </si>
-  <si>
-    <t>XTN</t>
-  </si>
-  <si>
-    <t>TEL</t>
-  </si>
-  <si>
     <t>CareTeam.note</t>
   </si>
   <si>
@@ -1261,12 +1202,6 @@
   </si>
   <si>
     <t>Comments made about the CareTeam.</t>
-  </si>
-  <si>
-    <t>For systems that do not have structured annotations, they can simply communicate a single annotation with no author or time.  This element may need to be included in narrative because of the potential for modifying information.  *Annotations SHOULD NOT* be used to communicate "modifying" information that could be computable. (This is a SHOULD because enforcing user behavior is nearly impossible).</t>
-  </si>
-  <si>
-    <t>Act</t>
   </si>
 </sst>
 </file>
@@ -1632,7 +1567,7 @@
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="37" max="37" width="36.91796875" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="155.80078125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="143.74609375" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="102.6171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2068,11 +2003,11 @@
         <v>85</v>
       </c>
       <c r="AI4" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ4" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ4" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK4" t="s" s="2">
         <v>76</v>
       </c>
@@ -2080,15 +2015,15 @@
         <v>76</v>
       </c>
       <c r="AM4" t="s" s="2">
-        <v>99</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
@@ -2111,13 +2046,13 @@
         <v>76</v>
       </c>
       <c r="K5" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="L5" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="M5" t="s" s="2">
         <v>101</v>
-      </c>
-      <c r="L5" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="M5" t="s" s="2">
-        <v>103</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -2168,7 +2103,7 @@
         <v>76</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>77</v>
@@ -2189,19 +2124,19 @@
         <v>76</v>
       </c>
       <c r="AM5" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
@@ -2220,16 +2155,16 @@
         <v>76</v>
       </c>
       <c r="K6" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="L6" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="M6" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="L6" t="s" s="2">
+      <c r="N6" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="M6" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="N6" t="s" s="2">
-        <v>111</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
@@ -2267,19 +2202,19 @@
         <v>76</v>
       </c>
       <c r="AB6" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AC6" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AD6" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE6" t="s" s="2">
         <v>112</v>
       </c>
-      <c r="AC6" t="s" s="2">
+      <c r="AF6" t="s" s="2">
         <v>113</v>
-      </c>
-      <c r="AD6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE6" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="AF6" t="s" s="2">
-        <v>115</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>77</v>
@@ -2288,10 +2223,10 @@
         <v>78</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AK6" t="s" s="2">
         <v>76</v>
@@ -2300,15 +2235,15 @@
         <v>76</v>
       </c>
       <c r="AM6" t="s" s="2">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
@@ -2334,13 +2269,13 @@
         <v>87</v>
       </c>
       <c r="L7" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="M7" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="N7" t="s" s="2">
         <v>118</v>
-      </c>
-      <c r="M7" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="N7" t="s" s="2">
-        <v>120</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" t="s" s="2">
@@ -2390,7 +2325,7 @@
         <v>76</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>77</v>
@@ -2399,11 +2334,11 @@
         <v>85</v>
       </c>
       <c r="AI7" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ7" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ7" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK7" t="s" s="2">
         <v>76</v>
       </c>
@@ -2411,15 +2346,15 @@
         <v>76</v>
       </c>
       <c r="AM7" t="s" s="2">
-        <v>105</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
@@ -2442,16 +2377,16 @@
         <v>86</v>
       </c>
       <c r="K8" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="L8" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="M8" t="s" s="2">
         <v>123</v>
       </c>
-      <c r="L8" t="s" s="2">
+      <c r="N8" t="s" s="2">
         <v>124</v>
-      </c>
-      <c r="M8" t="s" s="2">
-        <v>125</v>
-      </c>
-      <c r="N8" t="s" s="2">
-        <v>126</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
@@ -2501,7 +2436,7 @@
         <v>76</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AG8" t="s" s="2">
         <v>77</v>
@@ -2510,11 +2445,11 @@
         <v>85</v>
       </c>
       <c r="AI8" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ8" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ8" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK8" t="s" s="2">
         <v>76</v>
       </c>
@@ -2522,15 +2457,15 @@
         <v>76</v>
       </c>
       <c r="AM8" t="s" s="2">
-        <v>105</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
@@ -2553,16 +2488,16 @@
         <v>86</v>
       </c>
       <c r="K9" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="L9" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="M9" t="s" s="2">
         <v>129</v>
       </c>
-      <c r="L9" t="s" s="2">
+      <c r="N9" t="s" s="2">
         <v>130</v>
-      </c>
-      <c r="M9" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="N9" t="s" s="2">
-        <v>132</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" t="s" s="2">
@@ -2612,7 +2547,7 @@
         <v>76</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AG9" t="s" s="2">
         <v>77</v>
@@ -2621,11 +2556,11 @@
         <v>85</v>
       </c>
       <c r="AI9" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ9" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ9" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK9" t="s" s="2">
         <v>76</v>
       </c>
@@ -2633,15 +2568,15 @@
         <v>76</v>
       </c>
       <c r="AM9" t="s" s="2">
-        <v>105</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
@@ -2664,16 +2599,16 @@
         <v>86</v>
       </c>
       <c r="K10" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="L10" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="M10" t="s" s="2">
         <v>135</v>
       </c>
-      <c r="L10" t="s" s="2">
+      <c r="N10" t="s" s="2">
         <v>136</v>
-      </c>
-      <c r="M10" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="N10" t="s" s="2">
-        <v>138</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" t="s" s="2">
@@ -2723,7 +2658,7 @@
         <v>76</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>77</v>
@@ -2732,11 +2667,11 @@
         <v>78</v>
       </c>
       <c r="AI10" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ10" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ10" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK10" t="s" s="2">
         <v>76</v>
       </c>
@@ -2744,15 +2679,15 @@
         <v>76</v>
       </c>
       <c r="AM10" t="s" s="2">
-        <v>105</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
@@ -2775,16 +2710,16 @@
         <v>86</v>
       </c>
       <c r="K11" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="L11" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="M11" t="s" s="2">
         <v>141</v>
       </c>
-      <c r="L11" t="s" s="2">
+      <c r="N11" t="s" s="2">
         <v>142</v>
-      </c>
-      <c r="M11" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="N11" t="s" s="2">
-        <v>144</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" t="s" s="2">
@@ -2810,31 +2745,31 @@
         <v>76</v>
       </c>
       <c r="X11" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="Y11" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="Z11" t="s" s="2">
         <v>145</v>
       </c>
-      <c r="Y11" t="s" s="2">
+      <c r="AA11" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB11" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC11" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD11" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE11" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AF11" t="s" s="2">
         <v>146</v>
-      </c>
-      <c r="Z11" t="s" s="2">
-        <v>147</v>
-      </c>
-      <c r="AA11" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB11" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC11" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD11" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE11" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF11" t="s" s="2">
-        <v>148</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>77</v>
@@ -2843,27 +2778,27 @@
         <v>78</v>
       </c>
       <c r="AI11" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ11" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ11" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK11" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>149</v>
+        <v>76</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>150</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -2886,16 +2821,16 @@
         <v>86</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="N12" t="s" s="2">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="O12" s="2"/>
       <c r="P12" t="s" s="2">
@@ -2921,13 +2856,13 @@
         <v>76</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Z12" t="s" s="2">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="AA12" t="s" s="2">
         <v>76</v>
@@ -2945,7 +2880,7 @@
         <v>76</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>77</v>
@@ -2954,27 +2889,27 @@
         <v>78</v>
       </c>
       <c r="AI12" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ12" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ12" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK12" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>149</v>
+        <v>76</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>150</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -2997,16 +2932,16 @@
         <v>86</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" t="s" s="2">
@@ -3056,7 +2991,7 @@
         <v>76</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>77</v>
@@ -3065,11 +3000,11 @@
         <v>85</v>
       </c>
       <c r="AI13" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ13" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ13" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK13" t="s" s="2">
         <v>76</v>
       </c>
@@ -3077,15 +3012,15 @@
         <v>76</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>105</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -3108,16 +3043,16 @@
         <v>76</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="N14" t="s" s="2">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" t="s" s="2">
@@ -3143,13 +3078,13 @@
         <v>76</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="Z14" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AA14" t="s" s="2">
         <v>76</v>
@@ -3167,7 +3102,7 @@
         <v>76</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>77</v>
@@ -3176,11 +3111,11 @@
         <v>85</v>
       </c>
       <c r="AI14" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ14" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ14" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK14" t="s" s="2">
         <v>76</v>
       </c>
@@ -3188,19 +3123,19 @@
         <v>76</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>105</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" t="s" s="2">
@@ -3219,16 +3154,16 @@
         <v>76</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="O15" s="2"/>
       <c r="P15" t="s" s="2">
@@ -3278,7 +3213,7 @@
         <v>76</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>77</v>
@@ -3287,11 +3222,11 @@
         <v>85</v>
       </c>
       <c r="AI15" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ15" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ15" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK15" t="s" s="2">
         <v>76</v>
       </c>
@@ -3299,19 +3234,19 @@
         <v>76</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s" s="2">
@@ -3330,16 +3265,16 @@
         <v>76</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="O16" s="2"/>
       <c r="P16" t="s" s="2">
@@ -3389,7 +3324,7 @@
         <v>76</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>77</v>
@@ -3410,19 +3345,19 @@
         <v>76</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>99</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
@@ -3441,16 +3376,16 @@
         <v>76</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L17" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="M17" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="N17" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="M17" t="s" s="2">
-        <v>189</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>111</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" t="s" s="2">
@@ -3488,19 +3423,19 @@
         <v>76</v>
       </c>
       <c r="AB17" t="s" s="2">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="AC17" t="s" s="2">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="AD17" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>77</v>
@@ -3509,10 +3444,10 @@
         <v>78</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>76</v>
@@ -3521,19 +3456,19 @@
         <v>76</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>99</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" t="s" s="2">
@@ -3552,19 +3487,19 @@
         <v>76</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O18" t="s" s="2">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="P18" t="s" s="2">
         <v>76</v>
@@ -3601,19 +3536,19 @@
         <v>76</v>
       </c>
       <c r="AB18" t="s" s="2">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="AC18" t="s" s="2">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="AD18" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>77</v>
@@ -3622,10 +3557,10 @@
         <v>78</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>76</v>
@@ -3634,15 +3569,15 @@
         <v>76</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>99</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3665,19 +3600,19 @@
         <v>86</v>
       </c>
       <c r="K19" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="L19" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="M19" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="N19" t="s" s="2">
         <v>197</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="O19" t="s" s="2">
         <v>198</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="O19" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="P19" t="s" s="2">
         <v>76</v>
@@ -3726,7 +3661,7 @@
         <v>76</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>77</v>
@@ -3735,27 +3670,27 @@
         <v>78</v>
       </c>
       <c r="AI19" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ19" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ19" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK19" t="s" s="2">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>203</v>
+        <v>76</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>204</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3778,13 +3713,13 @@
         <v>76</v>
       </c>
       <c r="K20" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="L20" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="M20" t="s" s="2">
         <v>101</v>
-      </c>
-      <c r="L20" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>103</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -3835,7 +3770,7 @@
         <v>76</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>77</v>
@@ -3856,19 +3791,19 @@
         <v>76</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" t="s" s="2">
@@ -3887,16 +3822,16 @@
         <v>76</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="L21" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="M21" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="N21" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>111</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" t="s" s="2">
@@ -3934,19 +3869,19 @@
         <v>76</v>
       </c>
       <c r="AB21" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AC21" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AD21" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE21" t="s" s="2">
         <v>112</v>
       </c>
-      <c r="AC21" t="s" s="2">
+      <c r="AF21" t="s" s="2">
         <v>113</v>
-      </c>
-      <c r="AD21" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE21" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="AF21" t="s" s="2">
-        <v>115</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>77</v>
@@ -3955,10 +3890,10 @@
         <v>78</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>76</v>
@@ -3967,15 +3902,15 @@
         <v>76</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -3998,19 +3933,19 @@
         <v>86</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="O22" t="s" s="2">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="P22" t="s" s="2">
         <v>76</v>
@@ -4035,13 +3970,13 @@
         <v>76</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="Z22" t="s" s="2">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AA22" t="s" s="2">
         <v>76</v>
@@ -4059,7 +3994,7 @@
         <v>76</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>77</v>
@@ -4068,27 +4003,27 @@
         <v>85</v>
       </c>
       <c r="AI22" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ22" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ22" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK22" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>99</v>
+        <v>184</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4111,19 +4046,19 @@
         <v>86</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="O23" t="s" s="2">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="P23" t="s" s="2">
         <v>76</v>
@@ -4148,13 +4083,13 @@
         <v>76</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="Z23" t="s" s="2">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="AA23" t="s" s="2">
         <v>76</v>
@@ -4172,7 +4107,7 @@
         <v>76</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>77</v>
@@ -4181,27 +4116,27 @@
         <v>85</v>
       </c>
       <c r="AI23" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ23" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ23" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK23" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4224,19 +4159,19 @@
         <v>86</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="O24" t="s" s="2">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>76</v>
@@ -4249,7 +4184,7 @@
         <v>76</v>
       </c>
       <c r="T24" t="s" s="2">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="U24" t="s" s="2">
         <v>76</v>
@@ -4285,7 +4220,7 @@
         <v>76</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>77</v>
@@ -4294,27 +4229,27 @@
         <v>85</v>
       </c>
       <c r="AI24" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ24" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ24" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK24" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4337,19 +4272,19 @@
         <v>86</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="O25" t="s" s="2">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>76</v>
@@ -4362,7 +4297,7 @@
         <v>76</v>
       </c>
       <c r="T25" t="s" s="2">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="U25" t="s" s="2">
         <v>76</v>
@@ -4398,7 +4333,7 @@
         <v>76</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>77</v>
@@ -4407,27 +4342,27 @@
         <v>85</v>
       </c>
       <c r="AI25" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ25" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ25" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK25" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4450,17 +4385,15 @@
         <v>86</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>249</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" t="s" s="2">
         <v>76</v>
@@ -4509,7 +4442,7 @@
         <v>76</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>77</v>
@@ -4518,27 +4451,27 @@
         <v>85</v>
       </c>
       <c r="AI26" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ26" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ26" t="s" s="2">
-        <v>251</v>
-      </c>
       <c r="AK26" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4561,16 +4494,16 @@
         <v>86</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
@@ -4620,7 +4553,7 @@
         <v>76</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>77</v>
@@ -4629,27 +4562,27 @@
         <v>85</v>
       </c>
       <c r="AI27" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ27" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ27" t="s" s="2">
-        <v>260</v>
-      </c>
       <c r="AK27" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4672,16 +4605,16 @@
         <v>86</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -4707,13 +4640,13 @@
         <v>76</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="Z28" t="s" s="2">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>76</v>
@@ -4731,7 +4664,7 @@
         <v>76</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>77</v>
@@ -4740,27 +4673,27 @@
         <v>85</v>
       </c>
       <c r="AI28" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ28" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ28" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK28" t="s" s="2">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>105</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4783,19 +4716,19 @@
         <v>86</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="O29" t="s" s="2">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>76</v>
@@ -4820,13 +4753,13 @@
         <v>76</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="Z29" t="s" s="2">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="AA29" t="s" s="2">
         <v>76</v>
@@ -4844,7 +4777,7 @@
         <v>76</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>77</v>
@@ -4853,27 +4786,27 @@
         <v>78</v>
       </c>
       <c r="AI29" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ29" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK29" t="s" s="2">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>278</v>
+        <v>76</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>279</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4896,16 +4829,16 @@
         <v>86</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -4955,7 +4888,7 @@
         <v>76</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>77</v>
@@ -4964,11 +4897,11 @@
         <v>85</v>
       </c>
       <c r="AI30" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ30" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ30" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK30" t="s" s="2">
         <v>76</v>
       </c>
@@ -4976,19 +4909,19 @@
         <v>76</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>105</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
@@ -5007,19 +4940,17 @@
         <v>86</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>289</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>76</v>
@@ -5068,7 +4999,7 @@
         <v>76</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>77</v>
@@ -5077,27 +5008,27 @@
         <v>85</v>
       </c>
       <c r="AI31" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ31" t="s" s="2">
-        <v>260</v>
-      </c>
       <c r="AK31" t="s" s="2">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>292</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5120,16 +5051,16 @@
         <v>86</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
@@ -5179,7 +5110,7 @@
         <v>76</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>77</v>
@@ -5188,27 +5119,27 @@
         <v>85</v>
       </c>
       <c r="AI32" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ32" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ32" t="s" s="2">
-        <v>260</v>
-      </c>
       <c r="AK32" t="s" s="2">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>292</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5231,19 +5162,17 @@
         <v>86</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="N33" t="s" s="2">
-        <v>249</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="P33" t="s" s="2">
         <v>76</v>
@@ -5292,7 +5221,7 @@
         <v>76</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>77</v>
@@ -5301,27 +5230,27 @@
         <v>85</v>
       </c>
       <c r="AI33" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ33" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ33" t="s" s="2">
-        <v>251</v>
-      </c>
       <c r="AK33" t="s" s="2">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>304</v>
+        <v>76</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>305</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5344,13 +5273,13 @@
         <v>76</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="L34" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="M34" t="s" s="2">
         <v>101</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>103</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -5401,7 +5330,7 @@
         <v>76</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>77</v>
@@ -5422,19 +5351,19 @@
         <v>76</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5453,16 +5382,16 @@
         <v>76</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="L35" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="M35" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="N35" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>111</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -5500,19 +5429,19 @@
         <v>76</v>
       </c>
       <c r="AB35" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AC35" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AD35" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE35" t="s" s="2">
         <v>112</v>
       </c>
-      <c r="AC35" t="s" s="2">
+      <c r="AF35" t="s" s="2">
         <v>113</v>
-      </c>
-      <c r="AD35" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE35" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="AF35" t="s" s="2">
-        <v>115</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>77</v>
@@ -5521,10 +5450,10 @@
         <v>78</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>76</v>
@@ -5533,15 +5462,15 @@
         <v>76</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5564,16 +5493,16 @@
         <v>86</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="O36" s="2"/>
       <c r="P36" t="s" s="2">
@@ -5623,7 +5552,7 @@
         <v>76</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>77</v>
@@ -5632,27 +5561,27 @@
         <v>85</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5675,23 +5604,23 @@
         <v>86</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" t="s" s="2">
         <v>76</v>
       </c>
       <c r="Q37" t="s" s="2">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="R37" t="s" s="2">
         <v>76</v>
@@ -5736,7 +5665,7 @@
         <v>76</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>77</v>
@@ -5745,27 +5674,27 @@
         <v>85</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5788,16 +5717,16 @@
         <v>76</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="O38" s="2"/>
       <c r="P38" t="s" s="2">
@@ -5847,7 +5776,7 @@
         <v>76</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>77</v>
@@ -5856,27 +5785,27 @@
         <v>78</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>333</v>
+        <v>319</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -5899,13 +5828,13 @@
         <v>76</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="L39" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="M39" t="s" s="2">
         <v>101</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>103</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -5956,7 +5885,7 @@
         <v>76</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>77</v>
@@ -5977,19 +5906,19 @@
         <v>76</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
@@ -6008,16 +5937,16 @@
         <v>76</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="L40" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="M40" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="N40" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>111</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
@@ -6055,19 +5984,19 @@
         <v>76</v>
       </c>
       <c r="AB40" t="s" s="2">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="AC40" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD40" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE40" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AF40" t="s" s="2">
         <v>113</v>
-      </c>
-      <c r="AD40" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE40" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="AF40" t="s" s="2">
-        <v>115</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>77</v>
@@ -6076,10 +6005,10 @@
         <v>78</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>76</v>
@@ -6088,19 +6017,19 @@
         <v>76</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
@@ -6119,19 +6048,19 @@
         <v>86</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O41" t="s" s="2">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="P41" t="s" s="2">
         <v>76</v>
@@ -6180,7 +6109,7 @@
         <v>76</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>77</v>
@@ -6189,10 +6118,10 @@
         <v>78</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>76</v>
@@ -6201,15 +6130,15 @@
         <v>76</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>99</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6232,16 +6161,16 @@
         <v>86</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -6267,13 +6196,13 @@
         <v>76</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="Z42" t="s" s="2">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="AA42" t="s" s="2">
         <v>76</v>
@@ -6291,7 +6220,7 @@
         <v>76</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>77</v>
@@ -6300,27 +6229,27 @@
         <v>78</v>
       </c>
       <c r="AI42" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ42" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ42" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK42" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6343,19 +6272,19 @@
         <v>86</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="O43" t="s" s="2">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>76</v>
@@ -6404,7 +6333,7 @@
         <v>76</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>77</v>
@@ -6413,27 +6342,27 @@
         <v>85</v>
       </c>
       <c r="AI43" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ43" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ43" t="s" s="2">
-        <v>260</v>
-      </c>
       <c r="AK43" t="s" s="2">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>357</v>
+        <v>343</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6456,19 +6385,17 @@
         <v>86</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>289</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="P44" t="s" s="2">
         <v>76</v>
@@ -6517,7 +6444,7 @@
         <v>76</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>77</v>
@@ -6526,11 +6453,11 @@
         <v>85</v>
       </c>
       <c r="AI44" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ44" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ44" t="s" s="2">
-        <v>260</v>
-      </c>
       <c r="AK44" t="s" s="2">
         <v>76</v>
       </c>
@@ -6538,15 +6465,15 @@
         <v>76</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>292</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6569,16 +6496,16 @@
         <v>76</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -6628,7 +6555,7 @@
         <v>76</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>77</v>
@@ -6637,27 +6564,27 @@
         <v>85</v>
       </c>
       <c r="AI45" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ45" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ45" t="s" s="2">
-        <v>251</v>
-      </c>
       <c r="AK45" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>304</v>
+        <v>76</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>305</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6680,13 +6607,13 @@
         <v>76</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="L46" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="M46" t="s" s="2">
         <v>101</v>
-      </c>
-      <c r="L46" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>103</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -6737,7 +6664,7 @@
         <v>76</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>77</v>
@@ -6758,19 +6685,19 @@
         <v>76</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
@@ -6789,16 +6716,16 @@
         <v>76</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="L47" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="M47" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="L47" t="s" s="2">
+      <c r="N47" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="N47" t="s" s="2">
-        <v>111</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
@@ -6836,19 +6763,19 @@
         <v>76</v>
       </c>
       <c r="AB47" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AC47" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AD47" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE47" t="s" s="2">
         <v>112</v>
       </c>
-      <c r="AC47" t="s" s="2">
+      <c r="AF47" t="s" s="2">
         <v>113</v>
-      </c>
-      <c r="AD47" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE47" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="AF47" t="s" s="2">
-        <v>115</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>77</v>
@@ -6857,10 +6784,10 @@
         <v>78</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>76</v>
@@ -6869,15 +6796,15 @@
         <v>76</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -6900,16 +6827,16 @@
         <v>86</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
@@ -6959,7 +6886,7 @@
         <v>76</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>77</v>
@@ -6968,27 +6895,27 @@
         <v>85</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7011,23 +6938,23 @@
         <v>86</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="O49" s="2"/>
       <c r="P49" t="s" s="2">
         <v>76</v>
       </c>
       <c r="Q49" t="s" s="2">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="R49" t="s" s="2">
         <v>76</v>
@@ -7072,7 +6999,7 @@
         <v>76</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>77</v>
@@ -7081,27 +7008,27 @@
         <v>85</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7124,17 +7051,15 @@
         <v>76</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>375</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>376</v>
-      </c>
+        <v>361</v>
+      </c>
+      <c r="N50" s="2"/>
       <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
         <v>76</v>
@@ -7159,13 +7084,13 @@
         <v>76</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>377</v>
+        <v>362</v>
       </c>
       <c r="Z50" t="s" s="2">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="AA50" t="s" s="2">
         <v>76</v>
@@ -7183,7 +7108,7 @@
         <v>76</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>77</v>
@@ -7192,27 +7117,27 @@
         <v>78</v>
       </c>
       <c r="AI50" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ50" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ50" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK50" t="s" s="2">
-        <v>379</v>
+        <v>364</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>278</v>
+        <v>76</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>279</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7235,17 +7160,15 @@
         <v>76</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>382</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>289</v>
-      </c>
+        <v>367</v>
+      </c>
+      <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" t="s" s="2">
         <v>76</v>
@@ -7294,7 +7217,7 @@
         <v>76</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>77</v>
@@ -7303,27 +7226,27 @@
         <v>78</v>
       </c>
       <c r="AI51" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ51" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ51" t="s" s="2">
-        <v>260</v>
-      </c>
       <c r="AK51" t="s" s="2">
-        <v>379</v>
+        <v>364</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>292</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7346,19 +7269,17 @@
         <v>86</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>385</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>289</v>
-      </c>
+        <v>370</v>
+      </c>
+      <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="P52" t="s" s="2">
         <v>76</v>
@@ -7407,7 +7328,7 @@
         <v>76</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>77</v>
@@ -7416,11 +7337,11 @@
         <v>78</v>
       </c>
       <c r="AI52" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ52" t="s" s="2">
-        <v>260</v>
-      </c>
       <c r="AK52" t="s" s="2">
         <v>76</v>
       </c>
@@ -7428,15 +7349,15 @@
         <v>76</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>292</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7459,16 +7380,16 @@
         <v>76</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
@@ -7518,7 +7439,7 @@
         <v>76</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>77</v>
@@ -7527,27 +7448,27 @@
         <v>78</v>
       </c>
       <c r="AI53" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ53" t="s" s="2">
-        <v>392</v>
-      </c>
       <c r="AK53" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>393</v>
+        <v>76</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>394</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -7570,17 +7491,15 @@
         <v>76</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>396</v>
+        <v>378</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="N54" t="s" s="2">
-        <v>399</v>
-      </c>
+        <v>380</v>
+      </c>
+      <c r="N54" s="2"/>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
         <v>76</v>
@@ -7629,7 +7548,7 @@
         <v>76</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>77</v>
@@ -7638,19 +7557,19 @@
         <v>78</v>
       </c>
       <c r="AI54" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AJ54" t="s" s="2">
-        <v>98</v>
-      </c>
       <c r="AK54" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>400</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>